<commit_message>
Fixed error in batch mode
Corrected the function ParseParameterFile() to prevent occupancy output being selected if the landscape is artificial or if the number of replicates is 1
</commit_message>
<xml_diff>
--- a/doc/Manual/Batchmode/ParameterFile.xlsx
+++ b/doc/Manual/Batchmode/ParameterFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RangeShifter2\doc\Manual\Batchmode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25F8155-B1C5-4B70-993E-B7DCCE87A53E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF33D48-5E11-43C3-A873-624EEE186DCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="2" r:id="rId1"/>
@@ -195,9 +195,6 @@
     <t>Competition coefficient</t>
   </si>
   <si>
-    <t>Only if more than 1 replicate</t>
-  </si>
-  <si>
     <t xml:space="preserve">Save maps every  n reproductive seasons </t>
   </si>
   <si>
@@ -654,6 +651,9 @@
       </rPr>
       <t xml:space="preserve"> change in code numbers from v1</t>
     </r>
+  </si>
+  <si>
+    <t>Must be 0 for an artificial landscape or if there is only 1 replicate</t>
   </si>
 </sst>
 </file>
@@ -1798,763 +1798,763 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.6640625" style="25" customWidth="1"/>
-    <col min="4" max="4" width="58.5546875" style="25" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="11"/>
+    <col min="1" max="1" width="18.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.7109375" style="25" customWidth="1"/>
+    <col min="4" max="4" width="58.5703125" style="25" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>54</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>55</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:4" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="10"/>
-    </row>
-    <row r="4" spans="1:4" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>37</v>
-      </c>
       <c r="D4" s="10"/>
     </row>
-    <row r="5" spans="1:4" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="B5" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="34" t="s">
-        <v>113</v>
-      </c>
       <c r="D5" s="35"/>
     </row>
-    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>17</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D24" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="D29" s="36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30" s="37"/>
+    </row>
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="35"/>
+    </row>
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="35"/>
+    </row>
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" s="35"/>
+    </row>
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="27" t="s">
-        <v>118</v>
-      </c>
-      <c r="D29" s="36" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="D30" s="37"/>
-    </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B31" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C31" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="D31" s="35"/>
-    </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="B32" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="D32" s="35"/>
-    </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="B33" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C33" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="D33" s="35"/>
-    </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="B34" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C34" s="34" t="s">
+    </row>
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="D34" s="35" t="s">
+      <c r="B35" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" s="35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" s="35" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="B35" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C35" s="34" t="s">
-        <v>89</v>
-      </c>
-      <c r="D35" s="35" t="s">
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" s="35"/>
+    </row>
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="D39" s="35"/>
+    </row>
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" s="35"/>
+    </row>
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C41" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" s="35"/>
+    </row>
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B42" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D42" s="35"/>
+    </row>
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="B43" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="D43" s="35"/>
+    </row>
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="D44" s="35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C45" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="D45" s="35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="B46" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="D46" s="35" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="B36" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="D36" s="35" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="B37" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C37" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="D37" s="35"/>
-    </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="B38" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C38" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="D38" s="35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="B39" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C39" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="D39" s="35"/>
-    </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="B40" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C40" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="D40" s="35"/>
-    </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="B41" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C41" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="D41" s="35"/>
-    </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="32" t="s">
-        <v>114</v>
-      </c>
-      <c r="B42" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C42" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="D42" s="35"/>
-    </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="32" t="s">
-        <v>110</v>
-      </c>
-      <c r="B43" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C43" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="D43" s="35"/>
-    </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="B44" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C44" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="D44" s="35" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="B45" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C45" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="D45" s="35" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="B46" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="C46" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="D46" s="35" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D47" s="10"/>
     </row>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D48" s="10"/>
     </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D49" s="10"/>
     </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D50" s="10"/>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C51" s="24"/>
     </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C52" s="24"/>
     </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C53" s="24"/>
     </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C54" s="24"/>
     </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C55" s="24"/>
     </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C56" s="24"/>
     </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C57" s="24"/>
     </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C58" s="24"/>
     </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C59" s="24"/>
     </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C60" s="24"/>
     </row>
-    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C61" s="24"/>
     </row>
-    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C62" s="24"/>
     </row>
-    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C63" s="24"/>
     </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C64" s="24"/>
     </row>
-    <row r="65" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C65" s="24"/>
     </row>
-    <row r="66" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C66" s="24"/>
     </row>
-    <row r="67" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C67" s="24"/>
     </row>
-    <row r="68" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C68" s="24"/>
     </row>
-    <row r="69" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C69" s="24"/>
     </row>
-    <row r="70" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C70" s="24"/>
     </row>
-    <row r="71" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C71" s="24"/>
     </row>
-    <row r="72" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C72" s="24"/>
     </row>
-    <row r="73" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C73" s="24"/>
     </row>
-    <row r="74" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C74" s="24"/>
     </row>
-    <row r="75" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C75" s="24"/>
     </row>
-    <row r="76" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C76" s="24"/>
     </row>
-    <row r="77" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C77" s="24"/>
     </row>
-    <row r="78" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C78" s="24"/>
     </row>
   </sheetData>
@@ -2577,59 +2577,59 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="29" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="12.5546875" style="1" customWidth="1"/>
-    <col min="50" max="50" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="16384" width="9.109375" style="1"/>
+    <col min="35" max="35" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="12.5703125" style="1" customWidth="1"/>
+    <col min="50" max="50" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" s="28" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" s="28" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="28" t="s">
         <v>0</v>
@@ -2638,7 +2638,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E1" s="28" t="s">
         <v>2</v>
@@ -2671,7 +2671,7 @@
         <v>11</v>
       </c>
       <c r="O1" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P1" s="28" t="s">
         <v>12</v>
@@ -2698,73 +2698,73 @@
         <v>19</v>
       </c>
       <c r="X1" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Y1" s="28" t="s">
         <v>20</v>
       </c>
       <c r="Z1" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AA1" s="28" t="s">
         <v>21</v>
       </c>
       <c r="AB1" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AC1" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD1" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="AD1" s="30" t="s">
-        <v>72</v>
-      </c>
       <c r="AE1" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF1" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="AF1" s="31" t="s">
-        <v>82</v>
-      </c>
       <c r="AG1" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AH1" s="31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AI1" s="31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AJ1" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AK1" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AL1" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AM1" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AN1" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AO1" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AP1" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AQ1" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AR1" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AS1" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AT1" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AU1" s="31" t="s">
         <v>22</v>
@@ -2773,13 +2773,13 @@
         <v>23</v>
       </c>
       <c r="AW1" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AX1" s="31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>11</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>12</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>13</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>14</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>15</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>16</v>
       </c>
@@ -3860,59 +3860,59 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="12.5546875" style="1" customWidth="1"/>
-    <col min="48" max="48" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="16384" width="9.109375" style="1"/>
+    <col min="33" max="33" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="12.5703125" style="1" customWidth="1"/>
+    <col min="48" max="48" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -3921,7 +3921,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -3954,7 +3954,7 @@
         <v>11</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>12</v>
@@ -3981,67 +3981,67 @@
         <v>19</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Y1" s="3" t="s">
         <v>20</v>
       </c>
       <c r="Z1" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AA1" s="3" t="s">
         <v>21</v>
       </c>
       <c r="AB1" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AC1" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD1" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="AD1" s="31" t="s">
-        <v>82</v>
-      </c>
       <c r="AE1" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AF1" s="31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AG1" s="31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AH1" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AI1" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AJ1" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AK1" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AL1" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AM1" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AN1" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AO1" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AP1" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AQ1" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AR1" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AS1" s="31" t="s">
         <v>22</v>
@@ -4050,13 +4050,13 @@
         <v>23</v>
       </c>
       <c r="AU1" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AV1" s="31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -4202,7 +4202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>11</v>
       </c>
@@ -4348,7 +4348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>12</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>13</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>14</v>
       </c>
@@ -4786,7 +4786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>15</v>
       </c>
@@ -4932,7 +4932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>16</v>
       </c>
@@ -5094,58 +5094,58 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="12.5546875" style="1" customWidth="1"/>
-    <col min="48" max="48" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="16384" width="9.109375" style="1"/>
+    <col min="33" max="33" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="12.5703125" style="1" customWidth="1"/>
+    <col min="48" max="48" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -5154,7 +5154,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -5187,7 +5187,7 @@
         <v>11</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>12</v>
@@ -5214,67 +5214,67 @@
         <v>19</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Y1" s="3" t="s">
         <v>20</v>
       </c>
       <c r="Z1" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AA1" s="3" t="s">
         <v>21</v>
       </c>
       <c r="AB1" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AC1" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD1" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="AD1" s="31" t="s">
-        <v>82</v>
-      </c>
       <c r="AE1" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AF1" s="31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AG1" s="31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AH1" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AI1" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AJ1" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AK1" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AL1" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AM1" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AN1" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AO1" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AP1" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AQ1" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AR1" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AS1" s="31" t="s">
         <v>22</v>
@@ -5283,13 +5283,13 @@
         <v>23</v>
       </c>
       <c r="AU1" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AV1" s="31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -5435,7 +5435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>11</v>
       </c>
@@ -5581,7 +5581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>12</v>
       </c>
@@ -5727,7 +5727,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>13</v>
       </c>
@@ -5873,7 +5873,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>14</v>
       </c>
@@ -5980,7 +5980,7 @@
         <v>1</v>
       </c>
       <c r="AJ6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK6" s="1">
         <v>0</v>
@@ -6019,7 +6019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>15</v>
       </c>
@@ -6126,7 +6126,7 @@
         <v>1</v>
       </c>
       <c r="AJ7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK7" s="1">
         <v>0</v>
@@ -6165,7 +6165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>16</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v>1</v>
       </c>
       <c r="AJ8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK8" s="1">
         <v>0</v>

</xml_diff>